<commit_message>
Added some preliminary analysis
</commit_message>
<xml_diff>
--- a/nGoals.xlsx
+++ b/nGoals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2460" windowHeight="2550" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2460" windowHeight="2550" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GridMaps(Temp)" sheetId="6" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="36">
   <si>
     <t>ost001</t>
   </si>
@@ -206,6 +206,12 @@
   <si>
     <t>\kastar{}-\fmax{}</t>
   </si>
+  <si>
+    <t>\astar{} per goal</t>
+  </si>
+  <si>
+    <t>\kastar{}-\minf{}</t>
+  </si>
 </sst>
 </file>
 
@@ -284,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -309,12 +315,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="93">
+  <dxfs count="24">
     <dxf>
       <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
@@ -361,141 +373,6 @@
       <numFmt numFmtId="165" formatCode="0.0000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
@@ -503,78 +380,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -16175,63 +15980,63 @@
     <dataField name="Average of Denied" fld="6" subtotal="average" baseField="1" baseItem="4"/>
   </dataFields>
   <formats count="9">
-    <format dxfId="81">
+    <format dxfId="18">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="19">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="20">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="21">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="22">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="23">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="17">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="61">
+    <format dxfId="16">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="15">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
@@ -20989,10 +20794,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E20"/>
+  <dimension ref="A3:J48"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="A15:E20"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -21215,6 +21020,458 @@
         <v>1973420</v>
       </c>
     </row>
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="20">
+        <v>10</v>
+      </c>
+      <c r="B27" s="21">
+        <v>1.04192</v>
+      </c>
+      <c r="C27" s="21">
+        <v>0.52390599999999998</v>
+      </c>
+      <c r="D27" s="21">
+        <v>1063.3139999999999</v>
+      </c>
+      <c r="E27" s="21">
+        <v>1183.1759999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="19">
+        <v>1</v>
+      </c>
+      <c r="B28" s="17">
+        <v>8.7120000000000003E-2</v>
+      </c>
+      <c r="C28" s="17">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="D28" s="18">
+        <v>189.63</v>
+      </c>
+      <c r="E28" s="18">
+        <v>189.63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="19">
+        <v>2</v>
+      </c>
+      <c r="B29" s="17">
+        <v>0.20094000000000001</v>
+      </c>
+      <c r="C29" s="17">
+        <v>0.16145000000000001</v>
+      </c>
+      <c r="D29" s="18">
+        <v>363.06</v>
+      </c>
+      <c r="E29" s="18">
+        <v>368.19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="19">
+        <v>4</v>
+      </c>
+      <c r="B30" s="17">
+        <v>0.50541999999999998</v>
+      </c>
+      <c r="C30" s="17">
+        <v>0.34806999999999999</v>
+      </c>
+      <c r="D30" s="18">
+        <v>755.1</v>
+      </c>
+      <c r="E30" s="18">
+        <v>787.77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="19">
+        <v>8</v>
+      </c>
+      <c r="B31" s="17">
+        <v>1.1770400000000001</v>
+      </c>
+      <c r="C31" s="17">
+        <v>0.67479</v>
+      </c>
+      <c r="D31" s="18">
+        <v>1363.68</v>
+      </c>
+      <c r="E31" s="18">
+        <v>1511.91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="19">
+        <v>16</v>
+      </c>
+      <c r="B32" s="17">
+        <v>3.23908</v>
+      </c>
+      <c r="C32" s="17">
+        <v>1.35222</v>
+      </c>
+      <c r="D32" s="18">
+        <v>2645.1</v>
+      </c>
+      <c r="E32" s="18">
+        <v>3058.38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="20">
+        <v>20</v>
+      </c>
+      <c r="B33" s="22">
+        <v>61.679920000000003</v>
+      </c>
+      <c r="C33" s="22">
+        <v>23.073606000000002</v>
+      </c>
+      <c r="D33" s="23">
+        <v>40642.683999999994</v>
+      </c>
+      <c r="E33" s="23">
+        <v>41157.523999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="19">
+        <v>1</v>
+      </c>
+      <c r="B34" s="17">
+        <v>4.2441700000000004</v>
+      </c>
+      <c r="C34" s="17">
+        <v>4.1694000000000004</v>
+      </c>
+      <c r="D34" s="18">
+        <v>7324.12</v>
+      </c>
+      <c r="E34" s="18">
+        <v>7324.12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="19">
+        <v>2</v>
+      </c>
+      <c r="B35" s="17">
+        <v>9.7460299999999993</v>
+      </c>
+      <c r="C35" s="17">
+        <v>7.8148299999999997</v>
+      </c>
+      <c r="D35" s="18">
+        <v>13794</v>
+      </c>
+      <c r="E35" s="18">
+        <v>13828.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="19">
+        <v>4</v>
+      </c>
+      <c r="B36" s="17">
+        <v>21.742999999999999</v>
+      </c>
+      <c r="C36" s="17">
+        <v>13.7342</v>
+      </c>
+      <c r="D36" s="18">
+        <v>25153.7</v>
+      </c>
+      <c r="E36" s="18">
+        <v>24982</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="19">
+        <v>8</v>
+      </c>
+      <c r="B37" s="17">
+        <v>66.634399999999999</v>
+      </c>
+      <c r="C37" s="17">
+        <v>30.1389</v>
+      </c>
+      <c r="D37" s="18">
+        <v>53267.6</v>
+      </c>
+      <c r="E37" s="18">
+        <v>53790.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="19">
+        <v>16</v>
+      </c>
+      <c r="B38" s="17">
+        <v>206.03200000000001</v>
+      </c>
+      <c r="C38" s="17">
+        <v>59.5107</v>
+      </c>
+      <c r="D38" s="18">
+        <v>103674</v>
+      </c>
+      <c r="E38" s="18">
+        <v>105863</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="19">
+        <v>10</v>
+      </c>
+      <c r="F41">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="15"/>
+      <c r="B42" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J42" s="15"/>
+    </row>
+    <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I43" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J43" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="19">
+        <v>1</v>
+      </c>
+      <c r="B44" s="17">
+        <v>8.7120000000000003E-2</v>
+      </c>
+      <c r="C44" s="17">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="D44" s="18">
+        <v>189.63</v>
+      </c>
+      <c r="E44" s="18">
+        <v>189.63</v>
+      </c>
+      <c r="F44" s="19">
+        <v>1</v>
+      </c>
+      <c r="G44" s="17">
+        <v>4.2441700000000004</v>
+      </c>
+      <c r="H44" s="17">
+        <v>4.1694000000000004</v>
+      </c>
+      <c r="I44" s="18">
+        <v>7324.12</v>
+      </c>
+      <c r="J44" s="18">
+        <v>7324.12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="19">
+        <v>2</v>
+      </c>
+      <c r="B45" s="17">
+        <v>0.20094000000000001</v>
+      </c>
+      <c r="C45" s="17">
+        <v>0.16145000000000001</v>
+      </c>
+      <c r="D45" s="18">
+        <v>363.06</v>
+      </c>
+      <c r="E45" s="18">
+        <v>368.19</v>
+      </c>
+      <c r="F45" s="19">
+        <v>2</v>
+      </c>
+      <c r="G45" s="17">
+        <v>9.7460299999999993</v>
+      </c>
+      <c r="H45" s="17">
+        <v>7.8148299999999997</v>
+      </c>
+      <c r="I45" s="18">
+        <v>13794</v>
+      </c>
+      <c r="J45" s="18">
+        <v>13828.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="19">
+        <v>4</v>
+      </c>
+      <c r="B46" s="17">
+        <v>0.50541999999999998</v>
+      </c>
+      <c r="C46" s="17">
+        <v>0.34806999999999999</v>
+      </c>
+      <c r="D46" s="18">
+        <v>755.1</v>
+      </c>
+      <c r="E46" s="18">
+        <v>787.77</v>
+      </c>
+      <c r="F46" s="19">
+        <v>4</v>
+      </c>
+      <c r="G46" s="17">
+        <v>21.742999999999999</v>
+      </c>
+      <c r="H46" s="17">
+        <v>13.7342</v>
+      </c>
+      <c r="I46" s="18">
+        <v>25153.7</v>
+      </c>
+      <c r="J46" s="18">
+        <v>24982</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="19">
+        <v>8</v>
+      </c>
+      <c r="B47" s="17">
+        <v>1.1770400000000001</v>
+      </c>
+      <c r="C47" s="17">
+        <v>0.67479</v>
+      </c>
+      <c r="D47" s="18">
+        <v>1363.68</v>
+      </c>
+      <c r="E47" s="18">
+        <v>1511.91</v>
+      </c>
+      <c r="F47" s="19">
+        <v>8</v>
+      </c>
+      <c r="G47" s="17">
+        <v>66.634399999999999</v>
+      </c>
+      <c r="H47" s="17">
+        <v>30.1389</v>
+      </c>
+      <c r="I47" s="18">
+        <v>53267.6</v>
+      </c>
+      <c r="J47" s="18">
+        <v>53790.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="19">
+        <v>16</v>
+      </c>
+      <c r="B48" s="17">
+        <v>3.23908</v>
+      </c>
+      <c r="C48" s="17">
+        <v>1.35222</v>
+      </c>
+      <c r="D48" s="18">
+        <v>2645.1</v>
+      </c>
+      <c r="E48" s="18">
+        <v>3058.38</v>
+      </c>
+      <c r="F48" s="19">
+        <v>16</v>
+      </c>
+      <c r="G48" s="17">
+        <v>206.03200000000001</v>
+      </c>
+      <c r="H48" s="17">
+        <v>59.5107</v>
+      </c>
+      <c r="I48" s="18">
+        <v>103674</v>
+      </c>
+      <c r="J48" s="18">
+        <v>105863</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21224,17 +21481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E18"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" activeCellId="1" sqref="C5:C18 E5:E18"/>
-      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" axis="axisCol" dimension="1" start="3" min="2" max="4" activeRow="4" activeCol="4" previousRow="4" previousCol="4" click="1" r:id="rId1">
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="1" count="1">
-              <x v="1"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotSelection>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="A4:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>